<commit_message>
in german, add republicans
</commit_message>
<xml_diff>
--- a/Studies/CAMspiracy/t1_segmentation_German/static/Scale Brotherton et al., 2013/items Brotherton 2013.xlsx
+++ b/Studies/CAMspiracy/t1_segmentation_German/static/Scale Brotherton et al., 2013/items Brotherton 2013.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\labjsSoftware\article - CAMspiracy\t1_segmentation\static\Scale Brotherton et al., 2013\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\labjsSoftware\livmats studies\Studies\CAMspiracy\t1_segmentation_German\static\Scale Brotherton et al., 2013\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{47AFE2A4-628C-4324-A08F-EAFBC9DFD3D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3841159A-1FB8-4C27-AA3E-41A656685CAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Julius Fenn - Persönliche Ansicht" guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="2576" windowHeight="1416" activeSheetId="1"/>
+    <customWorkbookView name="Julius Fenn - Persönliche Ansicht" guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office-Anwender - Persönliche Ansicht" guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" mergeInterval="0" personalView="1" windowWidth="1365" windowHeight="704" activeSheetId="1"/>
     <customWorkbookView name="Philipp Höfele - Persönliche Ansicht" guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office-Anwender - Persönliche Ansicht" guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" mergeInterval="0" personalView="1" windowWidth="1365" windowHeight="704" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -37,51 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t xml:space="preserve">The government is involved in the murder of innocent citizens and/or well-known public figures, and keeps this a secret. </t>
-  </si>
-  <si>
-    <t>The power held by heads of state is second to that of small unknown groups who really control world politics.</t>
-  </si>
-  <si>
-    <t>Secret organizations communicate with extraterrestrials, but keep this fact from the public.</t>
-  </si>
-  <si>
-    <t>The spread of certain viruses and/or diseases is the result of the deliberate, concealed efforts of some organization.</t>
-  </si>
-  <si>
-    <t>Groups of scientists manipulate, fabricate, or suppress evidence in order to deceive the public.</t>
-  </si>
-  <si>
-    <t>The government permits or perpetrates acts of terrorism on its own soil, disguising its involvement.</t>
-  </si>
-  <si>
-    <t>A small, secret group of people is responsible for making all major world decisions, such as going to war.</t>
-  </si>
-  <si>
-    <t>Evidence of alien contact is being concealed from the public.</t>
-  </si>
-  <si>
-    <t>Technology with mind-control capacities is used on people without their knowledge.</t>
-  </si>
-  <si>
-    <t>New and advanced technology which would harm current industry is being suppressed.</t>
-  </si>
-  <si>
-    <t>The government uses people as patsies to hide its involvement in criminal activity.</t>
-  </si>
-  <si>
-    <t>Certain significant events have been the result of the activity of a small group who secretly manipulate world events.</t>
-  </si>
-  <si>
-    <t>Some UFO sightings and rumors are planned or staged in order to distract the public from real alien contact.</t>
-  </si>
-  <si>
-    <t>Experiments involving new drugs or technologies are routinely carried out on the public without their knowledge or consent.</t>
-  </si>
-  <si>
-    <t>A lot of important information is deliberately concealed from the public out of self-interest.</t>
-  </si>
   <si>
     <t>Number</t>
   </si>
@@ -133,6 +88,51 @@
   <si>
     <t>02et</t>
   </si>
+  <si>
+    <t>Die Regierung ist an Ermordungen unschuldiger Bürger und/oder bekannter Persönlichkeiten beteiligt, und hält diesen Sachverhalt geheim.</t>
+  </si>
+  <si>
+    <t>Die Macht von Staatsoberhäuptern ist der von kleinen anonymen Gruppen, die tatsächlich die Weltpolitik kontrollieren, untergeordnet.</t>
+  </si>
+  <si>
+    <t>Geheime Organisationen kommunizieren mit Außerirdischen, aber halten diese Tatsache vor der Öffentlichkeit zurück.</t>
+  </si>
+  <si>
+    <t>Die Verbreitung bestimmter Viren und/oder Krankheiten ist das Ergebnis der vorsätzlichen, verdeckten Aktionen einer Organisation.</t>
+  </si>
+  <si>
+    <t>Gruppen von Wissenschaftlern manipulieren, erfinden oder halten Beweise zurück, um die Öffentlichkeit zu täuschen.</t>
+  </si>
+  <si>
+    <t>Die Regierung erlaubt oder verübt selber terroristische Handlungen auf eigenem Grund und Boden und verschleiert dabei die eigene Beteiligung.</t>
+  </si>
+  <si>
+    <t>Ein kleiner, geheimer Personenkreis ist für das Treffen aller wichtigen Entscheidungen verantwortlich, wie z.B. in den Krieg zu ziehen.</t>
+  </si>
+  <si>
+    <t>Beweise für Kontakt mit Außerirdischen werden vor der Öffentlichkeit zurückgehalten.</t>
+  </si>
+  <si>
+    <t>Technologien, die im Stande sind Gedanken zu kontrollieren, werden an Menschen ohne deren Wissen eingesetzt.</t>
+  </si>
+  <si>
+    <t>Neue und fortschrittliche Technologien, die der gegenwärtigen Industrie schaden würden, werden zurückgehalten.</t>
+  </si>
+  <si>
+    <t>Die Regierung benutzt das Volk als Sündenbock, um die eigene Beteiligung an kriminellen Aktivitäten zu verbergen.</t>
+  </si>
+  <si>
+    <t>Gewisse bedeutende Ereignisse sind das Resultat der Aktivitäten einer kleinen Gruppe, die insgeheim das Weltgeschehen manipuliert.</t>
+  </si>
+  <si>
+    <t>Einige UFO-Sichtungen und -gerüchte werden geplant oder inszeniert, um die Öffentlichkeit von tatsächlich stattfindendem Kontakt mit Außerirdischen abzulenken.</t>
+  </si>
+  <si>
+    <t>Experimente, die mit neuen Medikamenten oder Technologien verbunden sind, werden regelmäßig an der Öffentlichkeit ohne deren Wissen oder Einverständnis durchgeführt.</t>
+  </si>
+  <si>
+    <t>Ein Großteil wichtiger Informationen wird aus Eigennutz absichtlich vor der Öffentlichkeit geheim gehalten.</t>
+  </si>
 </sst>
 </file>
 
@@ -167,13 +167,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -193,7 +194,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9FA9F96B-BE5F-42B8-854E-933B1D7481F5}" diskRevisions="1" revisionId="730" version="29">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A8D30B88-9E4F-4E13-97DB-C1ED21B64FDF}" diskRevisions="1" revisionId="761" version="30">
   <header guid="{09193A18-0B52-4FAB-B338-B4D967DC2D75}" dateTime="2022-09-29T13:56:20" maxSheetId="2" userName="Julius Fenn" r:id="rId23" minRId="265" maxRId="270">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -244,6 +245,11 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{A8D30B88-9E4F-4E13-97DB-C1ED21B64FDF}" dateTime="2023-11-25T17:47:21" maxSheetId="2" userName="Julius Fenn" r:id="rId33" minRId="731" maxRId="761">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -10323,7 +10329,653 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="731" sId="1" odxf="1" dxf="1">
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>Die Regierung ist an Ermordungen unschuldiger Bürger und/oder bekannter Persönlichkeiten beteiligt, und hält diesen Sachverhalt geheim.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="732" sId="1" odxf="1" dxf="1">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>Die Macht von Staatsoberhäuptern ist der von kleinen anonymen Gruppen, die tatsächlich die Weltpolitik kontrollieren, untergeordnet.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="733" sId="1" odxf="1" dxf="1">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <t>Geheime Organisationen kommunizieren mit Außerirdischen, aber halten diese Tatsache vor der Öffentlichkeit zurück.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="734" sId="1" odxf="1" dxf="1">
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Die Verbreitung bestimmter Viren und/oder Krankheiten ist das Ergebnis der vorsätzlichen, verdeckten Aktionen einer Organisation.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="735" sId="1" odxf="1" dxf="1">
+    <nc r="C6" t="inlineStr">
+      <is>
+        <t>Gruppen von Wissenschaftlern manipulieren, erfinden oder halten Beweise zurück, um die Öffentlichkeit zu täuschen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="736" sId="1" odxf="1" dxf="1">
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Die Regierung erlaubt oder verübt selber terroristische Handlungen auf eigenem Grund und Boden und verschleiert dabei die eigene Beteiligung.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="737" sId="1" odxf="1" dxf="1">
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Ein kleiner, geheimer Personenkreis ist für das Treffen aller wichtigen Entscheidungen verantwortlich, wie z.B. in den Krieg zu ziehen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="738" sId="1" odxf="1" dxf="1">
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Beweise für Kontakt mit Außerirdischen werden vor der Öffentlichkeit zurückgehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="739" sId="1" odxf="1" dxf="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Technologien, die im Stande sind Gedanken zu kontrollieren, werden an Menschen ohne deren Wissen eingesetzt.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="740" sId="1" odxf="1" dxf="1">
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>Neue und fortschrittliche Technologien, die der gegenwärtigen Industrie schaden würden, werden zurückgehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="741" sId="1" odxf="1" dxf="1">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Die Regierung benutzt das Volk als Sündenbock, um die eigene Beteiligung an kriminellen Aktivitäten zu verbergen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="742" sId="1" odxf="1" dxf="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Gewisse bedeutende Ereignisse sind das Resultat der Aktivitäten einer kleinen Gruppe, die insgeheim das Weltgeschehen manipuliert.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="743" sId="1" odxf="1" dxf="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Einige UFO-Sichtungen und -gerüchte werden geplant oder inszeniert, um die Öffentlichkeit von tatsächlich stattfindendem Kontakt mit Außerirdischen abzulenken.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="744" sId="1" odxf="1" dxf="1">
+    <nc r="C15" t="inlineStr">
+      <is>
+        <t>Experimente, die mit neuen Medikamenten oder Technologien verbunden sind, werden regelmäßig an der Öffentlichkeit ohne deren Wissen oder Einverständnis durchgeführt.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="745" sId="1" odxf="1" dxf="1">
+    <nc r="C16" t="inlineStr">
+      <is>
+        <t>Ein Großteil wichtiger Informationen wird aus Eigennutz absichtlich vor der Öffentlichkeit geheim gehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0"/>
+      <border outline="0">
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="746" sId="1" odxf="1" dxf="1">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t xml:space="preserve">The government is involved in the murder of innocent citizens and/or well-known public figures, and keeps this a secret. </t>
+      </is>
+    </oc>
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>Die Regierung ist an Ermordungen unschuldiger Bürger und/oder bekannter Persönlichkeiten beteiligt, und hält diesen Sachverhalt geheim.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="747" sId="1" odxf="1" dxf="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>The power held by heads of state is second to that of small unknown groups who really control world politics.</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>Die Macht von Staatsoberhäuptern ist der von kleinen anonymen Gruppen, die tatsächlich die Weltpolitik kontrollieren, untergeordnet.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="748" sId="1" odxf="1" dxf="1">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>Secret organizations communicate with extraterrestrials, but keep this fact from the public.</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>Geheime Organisationen kommunizieren mit Außerirdischen, aber halten diese Tatsache vor der Öffentlichkeit zurück.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="749" sId="1" odxf="1" dxf="1">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>The spread of certain viruses and/or diseases is the result of the deliberate, concealed efforts of some organization.</t>
+      </is>
+    </oc>
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>Die Verbreitung bestimmter Viren und/oder Krankheiten ist das Ergebnis der vorsätzlichen, verdeckten Aktionen einer Organisation.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="750" sId="1" odxf="1" dxf="1">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>Groups of scientists manipulate, fabricate, or suppress evidence in order to deceive the public.</t>
+      </is>
+    </oc>
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>Gruppen von Wissenschaftlern manipulieren, erfinden oder halten Beweise zurück, um die Öffentlichkeit zu täuschen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="751" sId="1" odxf="1" dxf="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>The government permits or perpetrates acts of terrorism on its own soil, disguising its involvement.</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>Die Regierung erlaubt oder verübt selber terroristische Handlungen auf eigenem Grund und Boden und verschleiert dabei die eigene Beteiligung.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="752" sId="1" odxf="1" dxf="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>A small, secret group of people is responsible for making all major world decisions, such as going to war.</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>Ein kleiner, geheimer Personenkreis ist für das Treffen aller wichtigen Entscheidungen verantwortlich, wie z.B. in den Krieg zu ziehen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="753" sId="1" odxf="1" dxf="1">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>Evidence of alien contact is being concealed from the public.</t>
+      </is>
+    </oc>
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>Beweise für Kontakt mit Außerirdischen werden vor der Öffentlichkeit zurückgehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="754" sId="1" odxf="1" dxf="1">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>Technology with mind-control capacities is used on people without their knowledge.</t>
+      </is>
+    </oc>
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>Technologien, die im Stande sind Gedanken zu kontrollieren, werden an Menschen ohne deren Wissen eingesetzt.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="755" sId="1" odxf="1" dxf="1">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>New and advanced technology which would harm current industry is being suppressed.</t>
+      </is>
+    </oc>
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>Neue und fortschrittliche Technologien, die der gegenwärtigen Industrie schaden würden, werden zurückgehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="756" sId="1" odxf="1" dxf="1">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>The government uses people as patsies to hide its involvement in criminal activity.</t>
+      </is>
+    </oc>
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>Die Regierung benutzt das Volk als Sündenbock, um die eigene Beteiligung an kriminellen Aktivitäten zu verbergen.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="757" sId="1" odxf="1" dxf="1">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>Certain significant events have been the result of the activity of a small group who secretly manipulate world events.</t>
+      </is>
+    </oc>
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>Gewisse bedeutende Ereignisse sind das Resultat der Aktivitäten einer kleinen Gruppe, die insgeheim das Weltgeschehen manipuliert.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="758" sId="1" odxf="1" dxf="1">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>Some UFO sightings and rumors are planned or staged in order to distract the public from real alien contact.</t>
+      </is>
+    </oc>
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>Einige UFO-Sichtungen und -gerüchte werden geplant oder inszeniert, um die Öffentlichkeit von tatsächlich stattfindendem Kontakt mit Außerirdischen abzulenken.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="759" sId="1" odxf="1" dxf="1">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>Experiments involving new drugs or technologies are routinely carried out on the public without their knowledge or consent.</t>
+      </is>
+    </oc>
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>Experimente, die mit neuen Medikamenten oder Technologien verbunden sind, werden regelmäßig an der Öffentlichkeit ohne deren Wissen oder Einverständnis durchgeführt.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="760" sId="1" odxf="1" dxf="1">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>A lot of important information is deliberately concealed from the public out of self-interest.</t>
+      </is>
+    </oc>
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>Ein Großteil wichtiger Informationen wird aus Eigennutz absichtlich vor der Öffentlichkeit geheim gehalten.</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment horizontal="left"/>
+      <border outline="0">
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <alignment horizontal="general"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rrc rId="761" sId="1" ref="C1:C1048576" action="deleteCol">
+    <rfmt sheetId="1" xfDxf="1" sqref="C1:C1048576" start="0" length="0"/>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C2" t="inlineStr">
+        <is>
+          <t>Die Regierung ist an Ermordungen unschuldiger Bürger und/oder bekannter Persönlichkeiten beteiligt, und hält diesen Sachverhalt geheim.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C3" t="inlineStr">
+        <is>
+          <t>Die Macht von Staatsoberhäuptern ist der von kleinen anonymen Gruppen, die tatsächlich die Weltpolitik kontrollieren, untergeordnet.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C4" t="inlineStr">
+        <is>
+          <t>Geheime Organisationen kommunizieren mit Außerirdischen, aber halten diese Tatsache vor der Öffentlichkeit zurück.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C5" t="inlineStr">
+        <is>
+          <t>Die Verbreitung bestimmter Viren und/oder Krankheiten ist das Ergebnis der vorsätzlichen, verdeckten Aktionen einer Organisation.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C6" t="inlineStr">
+        <is>
+          <t>Gruppen von Wissenschaftlern manipulieren, erfinden oder halten Beweise zurück, um die Öffentlichkeit zu täuschen.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>Die Regierung erlaubt oder verübt selber terroristische Handlungen auf eigenem Grund und Boden und verschleiert dabei die eigene Beteiligung.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C8" t="inlineStr">
+        <is>
+          <t>Ein kleiner, geheimer Personenkreis ist für das Treffen aller wichtigen Entscheidungen verantwortlich, wie z.B. in den Krieg zu ziehen.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C9" t="inlineStr">
+        <is>
+          <t>Beweise für Kontakt mit Außerirdischen werden vor der Öffentlichkeit zurückgehalten.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C10" t="inlineStr">
+        <is>
+          <t>Technologien, die im Stande sind Gedanken zu kontrollieren, werden an Menschen ohne deren Wissen eingesetzt.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C11" t="inlineStr">
+        <is>
+          <t>Neue und fortschrittliche Technologien, die der gegenwärtigen Industrie schaden würden, werden zurückgehalten.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C12" t="inlineStr">
+        <is>
+          <t>Die Regierung benutzt das Volk als Sündenbock, um die eigene Beteiligung an kriminellen Aktivitäten zu verbergen.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C13" t="inlineStr">
+        <is>
+          <t>Gewisse bedeutende Ereignisse sind das Resultat der Aktivitäten einer kleinen Gruppe, die insgeheim das Weltgeschehen manipuliert.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C14" t="inlineStr">
+        <is>
+          <t>Einige UFO-Sichtungen und -gerüchte werden geplant oder inszeniert, um die Öffentlichkeit von tatsächlich stattfindendem Kontakt mit Außerirdischen abzulenken.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C15" t="inlineStr">
+        <is>
+          <t>Experimente, die mit neuen Medikamenten oder Technologien verbunden sind, werden regelmäßig an der Öffentlichkeit ohne deren Wissen oder Einverständnis durchgeführt.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C16" t="inlineStr">
+        <is>
+          <t>Ein Großteil wichtiger Informationen wird aus Eigennutz absichtlich vor der Öffentlichkeit geheim gehalten.</t>
+        </is>
+      </nc>
+      <ndxf>
+        <alignment vertical="top" wrapText="1"/>
+        <border outline="0">
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+  </rrc>
+  <rcv guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" action="delete"/>
+  <rcv guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{09193A18-0B52-4FAB-B338-B4D967DC2D75}" name="Julius Fenn" id="-1936404097" dateTime="2022-09-29T13:55:36"/>
 </users>
@@ -10597,158 +11249,159 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
+      <c r="A13" s="1" t="s">
+        <v>7</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" scale="145" showPageBreaks="1" fitToPage="1" topLeftCell="A3">
-      <selection activeCell="F8" sqref="F8"/>
+    <customSheetView guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" scale="85" showPageBreaks="1" fitToPage="1">
+      <selection activeCell="B37" sqref="B37"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" scale="90" topLeftCell="B40">
-      <selection activeCell="F45" sqref="F45"/>
+    <customSheetView guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" scale="133" topLeftCell="A10">
+      <selection activeCell="E18" sqref="E18"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" scale="133" topLeftCell="A10">
-      <selection activeCell="E18" sqref="E18"/>
+    <customSheetView guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" scale="90" topLeftCell="B40">
+      <selection activeCell="F45" sqref="F45"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>